<commit_message>
Updated Pay Matrix file
</commit_message>
<xml_diff>
--- a/assets/pay matrix.xlsx
+++ b/assets/pay matrix.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PycharmProjects\pandasexcelproject\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LoKu\Desktop\Mutual Fund\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="vmrS4HYw/RzDLJlgzJAo9QTJNu3s0rPupc7mVPnY36AI79Ygu02tzGH5vVqrupII7I4zh+2lrS9ZP/eUy04p9g==" workbookSaltValue="CiJHBimjlaNOyBMQWjF3bQ==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDF45E0-FAB8-4169-AF18-834882D9A061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Pay Matrix ROPA 2009" sheetId="1" r:id="rId1"/>
+    <sheet name="Pay Matrix ROPA 2019" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Grade Pay</t>
   </si>
@@ -75,17 +75,20 @@
     <t>Information : This is the main Excel Pay Matrix file of the Pay Fixation Calculator Application. The app fetches required data from this sheet. Please do not modify this sheet.</t>
   </si>
   <si>
-    <t>Download : You can download the Automatic Pay Fixation Calculator from https://github.com/loku-sama/pay-fixation-wb</t>
+    <t>Contact : For any help email at loku-sama@outlook.com</t>
   </si>
   <si>
-    <t>Contact : For any help email at loku-sama@outlook.com</t>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>Download : You can download the Automatic Pay Fixation Calculator from :-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,14 +99,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -123,6 +118,23 @@
       <u/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -255,8 +267,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -264,9 +277,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -305,20 +315,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -596,11 +608,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,19 +661,19 @@
       <c r="K1" s="1">
         <v>9</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="8">
+      <c r="M1" s="7">
         <v>10</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="Q1" s="1">
@@ -670,10 +682,10 @@
       <c r="R1" s="1">
         <v>12</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="8" t="s">
         <v>9</v>
       </c>
       <c r="U1" s="1">
@@ -685,10 +697,10 @@
       <c r="W1" s="1">
         <v>15</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Y1" s="9" t="s">
         <v>11</v>
       </c>
       <c r="Z1" s="1">
@@ -703,7 +715,7 @@
       <c r="AC1" s="1">
         <v>19</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AD1" s="8" t="s">
         <v>12</v>
       </c>
       <c r="AE1" s="1">
@@ -721,10 +733,10 @@
       <c r="AI1" s="1">
         <v>24</v>
       </c>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="6"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
     </row>
-    <row r="2" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -746,7 +758,7 @@
       <c r="G2" s="2">
         <v>2600</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>2680</v>
       </c>
       <c r="I2" s="2">
@@ -758,19 +770,19 @@
       <c r="K2" s="2">
         <v>3600</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="3">
         <v>3650</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="3">
         <v>3900</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="3">
         <v>3950</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="3">
         <v>3960</v>
       </c>
-      <c r="P2" s="4">
+      <c r="P2" s="3">
         <v>4220</v>
       </c>
       <c r="Q2" s="2">
@@ -797,7 +809,7 @@
       <c r="X2" s="2">
         <v>5040</v>
       </c>
-      <c r="Y2" s="5">
+      <c r="Y2" s="4">
         <v>5640</v>
       </c>
       <c r="Z2" s="2">
@@ -830,10 +842,10 @@
       <c r="AI2" s="2">
         <v>10000</v>
       </c>
-      <c r="AJ2" s="6"/>
-      <c r="AK2" s="6"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
     </row>
-    <row r="3" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -855,7 +867,7 @@
       <c r="G3" s="2">
         <v>8840</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>9250</v>
       </c>
       <c r="I3" s="2">
@@ -867,19 +879,19 @@
       <c r="K3" s="2">
         <v>11040</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="3">
         <v>12120</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="3">
         <v>12270</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="3">
         <v>12600</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3" s="3">
         <v>13170</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P3" s="3">
         <v>15940</v>
       </c>
       <c r="Q3" s="2">
@@ -906,7 +918,7 @@
       <c r="X3" s="2">
         <v>19550</v>
       </c>
-      <c r="Y3" s="5">
+      <c r="Y3" s="4">
         <v>22570</v>
       </c>
       <c r="Z3" s="2">
@@ -939,8 +951,8 @@
       <c r="AI3" s="2">
         <v>47400</v>
       </c>
-      <c r="AJ3" s="6"/>
-      <c r="AK3" s="6"/>
+      <c r="AJ3" s="5"/>
+      <c r="AK3" s="5"/>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1048,11 +1060,11 @@
       <c r="AI4" s="1">
         <v>34</v>
       </c>
-      <c r="AJ4" s="6"/>
-      <c r="AK4" s="6"/>
+      <c r="AJ4" s="5"/>
+      <c r="AK4" s="5"/>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>1</v>
       </c>
       <c r="B5" s="2">
@@ -1073,31 +1085,31 @@
       <c r="G5" s="2">
         <v>22700</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="11">
         <v>23800</v>
       </c>
       <c r="I5" s="2">
         <v>24700</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="11">
         <v>27000</v>
       </c>
       <c r="K5" s="2">
         <v>28900</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="12">
         <v>31800</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="3">
         <v>32100</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5" s="12">
         <v>33000</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="12">
         <v>34500</v>
       </c>
-      <c r="P5" s="18">
+      <c r="P5" s="17">
         <v>41800</v>
       </c>
       <c r="Q5" s="2">
@@ -1106,10 +1118,10 @@
       <c r="R5" s="2">
         <v>35800</v>
       </c>
-      <c r="S5" s="12">
+      <c r="S5" s="11">
         <v>39500</v>
       </c>
-      <c r="T5" s="12">
+      <c r="T5" s="11">
         <v>44800</v>
       </c>
       <c r="U5" s="2">
@@ -1121,10 +1133,10 @@
       <c r="W5" s="2">
         <v>42600</v>
       </c>
-      <c r="X5" s="12">
+      <c r="X5" s="11">
         <v>52200</v>
       </c>
-      <c r="Y5" s="14">
+      <c r="Y5" s="13">
         <v>60300</v>
       </c>
       <c r="Z5" s="2">
@@ -1139,7 +1151,7 @@
       <c r="AC5" s="2">
         <v>95100</v>
       </c>
-      <c r="AD5" s="12">
+      <c r="AD5" s="11">
         <v>95400</v>
       </c>
       <c r="AE5" s="2">
@@ -1157,20 +1169,20 @@
       <c r="AI5" s="2">
         <v>128900</v>
       </c>
-      <c r="AJ5" s="6"/>
-      <c r="AK5" s="6"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>2</v>
       </c>
       <c r="B6" s="2">
         <v>17500</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>18100</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>19400</v>
       </c>
       <c r="E6" s="2">
@@ -1206,7 +1218,7 @@
       <c r="O6" s="2">
         <v>35500</v>
       </c>
-      <c r="P6" s="19">
+      <c r="P6" s="18">
         <v>43100</v>
       </c>
       <c r="Q6" s="2">
@@ -1266,20 +1278,20 @@
       <c r="AI6" s="2">
         <v>132800</v>
       </c>
-      <c r="AJ6" s="6"/>
-      <c r="AK6" s="6"/>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="5"/>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>3</v>
       </c>
       <c r="B7" s="2">
         <v>18000</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>18600</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>20000</v>
       </c>
       <c r="E7" s="2">
@@ -1315,7 +1327,7 @@
       <c r="O7" s="2">
         <v>36600</v>
       </c>
-      <c r="P7" s="19">
+      <c r="P7" s="18">
         <v>44400</v>
       </c>
       <c r="Q7" s="2">
@@ -1375,20 +1387,20 @@
       <c r="AI7" s="2">
         <v>136800</v>
       </c>
-      <c r="AJ7" s="6"/>
-      <c r="AK7" s="6"/>
+      <c r="AJ7" s="5"/>
+      <c r="AK7" s="5"/>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+      <c r="A8" s="10">
         <v>4</v>
       </c>
       <c r="B8" s="2">
         <v>18500</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>19200</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>20600</v>
       </c>
       <c r="E8" s="2">
@@ -1424,7 +1436,7 @@
       <c r="O8" s="2">
         <v>37700</v>
       </c>
-      <c r="P8" s="19">
+      <c r="P8" s="18">
         <v>45700</v>
       </c>
       <c r="Q8" s="2">
@@ -1484,20 +1496,20 @@
       <c r="AI8" s="2">
         <v>140900</v>
       </c>
-      <c r="AJ8" s="6"/>
-      <c r="AK8" s="6"/>
+      <c r="AJ8" s="5"/>
+      <c r="AK8" s="5"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+      <c r="A9" s="10">
         <v>5</v>
       </c>
       <c r="B9" s="2">
         <v>19100</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>19800</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>21200</v>
       </c>
       <c r="E9" s="2">
@@ -1533,7 +1545,7 @@
       <c r="O9" s="2">
         <v>38800</v>
       </c>
-      <c r="P9" s="19">
+      <c r="P9" s="18">
         <v>47100</v>
       </c>
       <c r="Q9" s="2">
@@ -1593,20 +1605,20 @@
       <c r="AI9" s="2">
         <v>145100</v>
       </c>
-      <c r="AJ9" s="6"/>
-      <c r="AK9" s="6"/>
+      <c r="AJ9" s="5"/>
+      <c r="AK9" s="5"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>6</v>
       </c>
       <c r="B10" s="2">
         <v>19700</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>20400</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>21800</v>
       </c>
       <c r="E10" s="2">
@@ -1642,7 +1654,7 @@
       <c r="O10" s="2">
         <v>40000</v>
       </c>
-      <c r="P10" s="19">
+      <c r="P10" s="18">
         <v>48500</v>
       </c>
       <c r="Q10" s="2">
@@ -1702,20 +1714,20 @@
       <c r="AI10" s="2">
         <v>149500</v>
       </c>
-      <c r="AJ10" s="6"/>
-      <c r="AK10" s="6"/>
+      <c r="AJ10" s="5"/>
+      <c r="AK10" s="5"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="A11" s="10">
         <v>7</v>
       </c>
       <c r="B11" s="2">
         <v>20300</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>21000</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>22500</v>
       </c>
       <c r="E11" s="2">
@@ -1751,7 +1763,7 @@
       <c r="O11" s="2">
         <v>41200</v>
       </c>
-      <c r="P11" s="19">
+      <c r="P11" s="18">
         <v>50000</v>
       </c>
       <c r="Q11" s="2">
@@ -1811,20 +1823,20 @@
       <c r="AI11" s="2">
         <v>154000</v>
       </c>
-      <c r="AJ11" s="6"/>
-      <c r="AK11" s="6"/>
+      <c r="AJ11" s="5"/>
+      <c r="AK11" s="5"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+      <c r="A12" s="10">
         <v>8</v>
       </c>
       <c r="B12" s="2">
         <v>20900</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>21600</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>23200</v>
       </c>
       <c r="E12" s="2">
@@ -1860,7 +1872,7 @@
       <c r="O12" s="2">
         <v>42400</v>
       </c>
-      <c r="P12" s="19">
+      <c r="P12" s="18">
         <v>51500</v>
       </c>
       <c r="Q12" s="2">
@@ -1920,20 +1932,20 @@
       <c r="AI12" s="2">
         <v>158600</v>
       </c>
-      <c r="AJ12" s="6"/>
-      <c r="AK12" s="6"/>
+      <c r="AJ12" s="5"/>
+      <c r="AK12" s="5"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+      <c r="A13" s="10">
         <v>9</v>
       </c>
       <c r="B13" s="2">
         <v>21500</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>22200</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>23900</v>
       </c>
       <c r="E13" s="2">
@@ -1969,7 +1981,7 @@
       <c r="O13" s="2">
         <v>43700</v>
       </c>
-      <c r="P13" s="19">
+      <c r="P13" s="18">
         <v>53000</v>
       </c>
       <c r="Q13" s="2">
@@ -2029,20 +2041,20 @@
       <c r="AI13" s="2">
         <v>163400</v>
       </c>
-      <c r="AJ13" s="6"/>
-      <c r="AK13" s="6"/>
+      <c r="AJ13" s="5"/>
+      <c r="AK13" s="5"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="A14" s="10">
         <v>10</v>
       </c>
       <c r="B14" s="2">
         <v>22100</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>22900</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>24600</v>
       </c>
       <c r="E14" s="2">
@@ -2078,7 +2090,7 @@
       <c r="O14" s="2">
         <v>45000</v>
       </c>
-      <c r="P14" s="19">
+      <c r="P14" s="18">
         <v>54600</v>
       </c>
       <c r="Q14" s="2">
@@ -2138,20 +2150,20 @@
       <c r="AI14" s="2">
         <v>168300</v>
       </c>
-      <c r="AJ14" s="6"/>
-      <c r="AK14" s="6"/>
+      <c r="AJ14" s="5"/>
+      <c r="AK14" s="5"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
+      <c r="A15" s="10">
         <v>11</v>
       </c>
       <c r="B15" s="2">
         <v>22800</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>23600</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>25300</v>
       </c>
       <c r="E15" s="2">
@@ -2187,7 +2199,7 @@
       <c r="O15" s="2">
         <v>46400</v>
       </c>
-      <c r="P15" s="19">
+      <c r="P15" s="18">
         <v>56200</v>
       </c>
       <c r="Q15" s="2">
@@ -2247,20 +2259,20 @@
       <c r="AI15" s="2">
         <v>173300</v>
       </c>
-      <c r="AJ15" s="6"/>
-      <c r="AK15" s="6"/>
+      <c r="AJ15" s="5"/>
+      <c r="AK15" s="5"/>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
+      <c r="A16" s="10">
         <v>12</v>
       </c>
       <c r="B16" s="2">
         <v>23500</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>24300</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>26100</v>
       </c>
       <c r="E16" s="2">
@@ -2278,7 +2290,7 @@
       <c r="I16" s="2">
         <v>34200</v>
       </c>
-      <c r="J16" s="15">
+      <c r="J16" s="14">
         <v>37400</v>
       </c>
       <c r="K16" s="2">
@@ -2296,7 +2308,7 @@
       <c r="O16" s="2">
         <v>47800</v>
       </c>
-      <c r="P16" s="19">
+      <c r="P16" s="18">
         <v>57900</v>
       </c>
       <c r="Q16" s="2">
@@ -2356,20 +2368,20 @@
       <c r="AI16" s="2">
         <v>178500</v>
       </c>
-      <c r="AJ16" s="6"/>
-      <c r="AK16" s="6"/>
+      <c r="AJ16" s="5"/>
+      <c r="AK16" s="5"/>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
+      <c r="A17" s="10">
         <v>13</v>
       </c>
       <c r="B17" s="2">
         <v>24200</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>25000</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>26900</v>
       </c>
       <c r="E17" s="2">
@@ -2405,7 +2417,7 @@
       <c r="O17" s="2">
         <v>49200</v>
       </c>
-      <c r="P17" s="19">
+      <c r="P17" s="18">
         <v>59600</v>
       </c>
       <c r="Q17" s="2">
@@ -2465,20 +2477,20 @@
       <c r="AI17" s="2">
         <v>183900</v>
       </c>
-      <c r="AJ17" s="6"/>
-      <c r="AK17" s="6"/>
+      <c r="AJ17" s="5"/>
+      <c r="AK17" s="5"/>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
+      <c r="A18" s="10">
         <v>14</v>
       </c>
       <c r="B18" s="2">
         <v>24900</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>25800</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <v>27700</v>
       </c>
       <c r="E18" s="2">
@@ -2514,7 +2526,7 @@
       <c r="O18" s="2">
         <v>50700</v>
       </c>
-      <c r="P18" s="19">
+      <c r="P18" s="18">
         <v>61400</v>
       </c>
       <c r="Q18" s="2">
@@ -2574,20 +2586,20 @@
       <c r="AI18" s="2">
         <v>189400</v>
       </c>
-      <c r="AJ18" s="6"/>
-      <c r="AK18" s="6"/>
+      <c r="AJ18" s="5"/>
+      <c r="AK18" s="5"/>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
+      <c r="A19" s="10">
         <v>15</v>
       </c>
       <c r="B19" s="2">
         <v>25600</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>26600</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="3">
         <v>28500</v>
       </c>
       <c r="E19" s="2">
@@ -2623,7 +2635,7 @@
       <c r="O19" s="2">
         <v>52200</v>
       </c>
-      <c r="P19" s="19">
+      <c r="P19" s="18">
         <v>63200</v>
       </c>
       <c r="Q19" s="2">
@@ -2683,20 +2695,20 @@
       <c r="AI19" s="2">
         <v>195100</v>
       </c>
-      <c r="AJ19" s="6"/>
-      <c r="AK19" s="6"/>
+      <c r="AJ19" s="5"/>
+      <c r="AK19" s="5"/>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
+      <c r="A20" s="10">
         <v>16</v>
       </c>
       <c r="B20" s="2">
         <v>26400</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>27400</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <v>29400</v>
       </c>
       <c r="E20" s="2">
@@ -2732,7 +2744,7 @@
       <c r="O20" s="2">
         <v>53800</v>
       </c>
-      <c r="P20" s="19">
+      <c r="P20" s="18">
         <v>65100</v>
       </c>
       <c r="Q20" s="2">
@@ -2792,20 +2804,20 @@
       <c r="AI20" s="2">
         <v>201000</v>
       </c>
-      <c r="AJ20" s="6"/>
-      <c r="AK20" s="6"/>
+      <c r="AJ20" s="5"/>
+      <c r="AK20" s="5"/>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
+      <c r="A21" s="10">
         <v>17</v>
       </c>
       <c r="B21" s="2">
         <v>27200</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>28200</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>30300</v>
       </c>
       <c r="E21" s="2">
@@ -2841,7 +2853,7 @@
       <c r="O21" s="2">
         <v>55400</v>
       </c>
-      <c r="P21" s="19">
+      <c r="P21" s="18">
         <v>67100</v>
       </c>
       <c r="Q21" s="2">
@@ -2893,20 +2905,20 @@
       <c r="AG21" s="2"/>
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
-      <c r="AJ21" s="6"/>
-      <c r="AK21" s="6"/>
+      <c r="AJ21" s="5"/>
+      <c r="AK21" s="5"/>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
+      <c r="A22" s="10">
         <v>18</v>
       </c>
       <c r="B22" s="2">
         <v>28000</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>29000</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>31200</v>
       </c>
       <c r="E22" s="2">
@@ -2942,7 +2954,7 @@
       <c r="O22" s="2">
         <v>57100</v>
       </c>
-      <c r="P22" s="19">
+      <c r="P22" s="18">
         <v>69100</v>
       </c>
       <c r="Q22" s="2">
@@ -2994,20 +3006,20 @@
       <c r="AG22" s="2"/>
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
-      <c r="AJ22" s="6"/>
-      <c r="AK22" s="6"/>
+      <c r="AJ22" s="5"/>
+      <c r="AK22" s="5"/>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
+      <c r="A23" s="10">
         <v>19</v>
       </c>
       <c r="B23" s="2">
         <v>28800</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <v>29900</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <v>32100</v>
       </c>
       <c r="E23" s="2">
@@ -3043,7 +3055,7 @@
       <c r="O23" s="2">
         <v>58800</v>
       </c>
-      <c r="P23" s="19">
+      <c r="P23" s="18">
         <v>71200</v>
       </c>
       <c r="Q23" s="2">
@@ -3095,20 +3107,20 @@
       <c r="AG23" s="2"/>
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
-      <c r="AJ23" s="6"/>
-      <c r="AK23" s="6"/>
+      <c r="AJ23" s="5"/>
+      <c r="AK23" s="5"/>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
+      <c r="A24" s="10">
         <v>20</v>
       </c>
       <c r="B24" s="2">
         <v>29700</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>30800</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <v>33100</v>
       </c>
       <c r="E24" s="2">
@@ -3144,7 +3156,7 @@
       <c r="O24" s="2">
         <v>60600</v>
       </c>
-      <c r="P24" s="19">
+      <c r="P24" s="18">
         <v>73300</v>
       </c>
       <c r="Q24" s="2">
@@ -3194,20 +3206,20 @@
       <c r="AG24" s="2"/>
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
-      <c r="AJ24" s="6"/>
-      <c r="AK24" s="6"/>
+      <c r="AJ24" s="5"/>
+      <c r="AK24" s="5"/>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
+      <c r="A25" s="10">
         <v>21</v>
       </c>
       <c r="B25" s="2">
         <v>30600</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <v>31700</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="3">
         <v>34100</v>
       </c>
       <c r="E25" s="2">
@@ -3243,7 +3255,7 @@
       <c r="O25" s="2">
         <v>62400</v>
       </c>
-      <c r="P25" s="19">
+      <c r="P25" s="18">
         <v>75500</v>
       </c>
       <c r="Q25" s="2">
@@ -3293,20 +3305,20 @@
       <c r="AG25" s="2"/>
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
-      <c r="AJ25" s="6"/>
-      <c r="AK25" s="6"/>
+      <c r="AJ25" s="5"/>
+      <c r="AK25" s="5"/>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
+      <c r="A26" s="10">
         <v>22</v>
       </c>
       <c r="B26" s="2">
         <v>31500</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="3">
         <v>32700</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="3">
         <v>35100</v>
       </c>
       <c r="E26" s="2">
@@ -3342,7 +3354,7 @@
       <c r="O26" s="2">
         <v>64300</v>
       </c>
-      <c r="P26" s="19">
+      <c r="P26" s="18">
         <v>77800</v>
       </c>
       <c r="Q26" s="2">
@@ -3392,20 +3404,20 @@
       <c r="AG26" s="2"/>
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
-      <c r="AJ26" s="6"/>
-      <c r="AK26" s="6"/>
+      <c r="AJ26" s="5"/>
+      <c r="AK26" s="5"/>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A27" s="11">
+      <c r="A27" s="10">
         <v>23</v>
       </c>
       <c r="B27" s="2">
         <v>32400</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="3">
         <v>33700</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="3">
         <v>36200</v>
       </c>
       <c r="E27" s="2">
@@ -3441,7 +3453,7 @@
       <c r="O27" s="2">
         <v>66200</v>
       </c>
-      <c r="P27" s="19">
+      <c r="P27" s="18">
         <v>80100</v>
       </c>
       <c r="Q27" s="2">
@@ -3491,20 +3503,20 @@
       <c r="AG27" s="2"/>
       <c r="AH27" s="2"/>
       <c r="AI27" s="2"/>
-      <c r="AJ27" s="6"/>
-      <c r="AK27" s="6"/>
+      <c r="AJ27" s="5"/>
+      <c r="AK27" s="5"/>
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A28" s="11">
+      <c r="A28" s="10">
         <v>24</v>
       </c>
       <c r="B28" s="2">
         <v>33400</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="3">
         <v>34700</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="3">
         <v>37300</v>
       </c>
       <c r="E28" s="2">
@@ -3540,7 +3552,7 @@
       <c r="O28" s="2">
         <v>68200</v>
       </c>
-      <c r="P28" s="19">
+      <c r="P28" s="18">
         <v>82500</v>
       </c>
       <c r="Q28" s="2">
@@ -3586,20 +3598,20 @@
       <c r="AG28" s="2"/>
       <c r="AH28" s="2"/>
       <c r="AI28" s="2"/>
-      <c r="AJ28" s="6"/>
-      <c r="AK28" s="6"/>
+      <c r="AJ28" s="5"/>
+      <c r="AK28" s="5"/>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A29" s="11">
+      <c r="A29" s="10">
         <v>25</v>
       </c>
       <c r="B29" s="2">
         <v>34400</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="3">
         <v>35700</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="3">
         <v>38400</v>
       </c>
       <c r="E29" s="2">
@@ -3635,7 +3647,7 @@
       <c r="O29" s="2">
         <v>70200</v>
       </c>
-      <c r="P29" s="19">
+      <c r="P29" s="18">
         <v>85000</v>
       </c>
       <c r="Q29" s="2">
@@ -3681,20 +3693,20 @@
       <c r="AG29" s="2"/>
       <c r="AH29" s="2"/>
       <c r="AI29" s="2"/>
-      <c r="AJ29" s="6"/>
-      <c r="AK29" s="6"/>
+      <c r="AJ29" s="5"/>
+      <c r="AK29" s="5"/>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A30" s="11">
+      <c r="A30" s="10">
         <v>26</v>
       </c>
       <c r="B30" s="2">
         <v>35400</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="3">
         <v>36800</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="3">
         <v>39600</v>
       </c>
       <c r="E30" s="2">
@@ -3730,7 +3742,7 @@
       <c r="O30" s="2">
         <v>72300</v>
       </c>
-      <c r="P30" s="19">
+      <c r="P30" s="18">
         <v>87600</v>
       </c>
       <c r="Q30" s="2">
@@ -3776,20 +3788,20 @@
       <c r="AG30" s="2"/>
       <c r="AH30" s="2"/>
       <c r="AI30" s="2"/>
-      <c r="AJ30" s="6"/>
-      <c r="AK30" s="6"/>
+      <c r="AJ30" s="5"/>
+      <c r="AK30" s="5"/>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A31" s="11">
+      <c r="A31" s="10">
         <v>27</v>
       </c>
       <c r="B31" s="2">
         <v>36500</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="3">
         <v>37900</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="3">
         <v>40800</v>
       </c>
       <c r="E31" s="2">
@@ -3825,7 +3837,7 @@
       <c r="O31" s="2">
         <v>74500</v>
       </c>
-      <c r="P31" s="19">
+      <c r="P31" s="18">
         <v>90200</v>
       </c>
       <c r="Q31" s="2">
@@ -3871,20 +3883,20 @@
       <c r="AG31" s="2"/>
       <c r="AH31" s="2"/>
       <c r="AI31" s="2"/>
-      <c r="AJ31" s="6"/>
-      <c r="AK31" s="6"/>
+      <c r="AJ31" s="5"/>
+      <c r="AK31" s="5"/>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A32" s="11">
+      <c r="A32" s="10">
         <v>28</v>
       </c>
       <c r="B32" s="2">
         <v>37600</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>39000</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="3">
         <v>42000</v>
       </c>
       <c r="E32" s="2">
@@ -3920,7 +3932,7 @@
       <c r="O32" s="2">
         <v>76700</v>
       </c>
-      <c r="P32" s="19">
+      <c r="P32" s="18">
         <v>92900</v>
       </c>
       <c r="Q32" s="2">
@@ -3966,20 +3978,20 @@
       <c r="AG32" s="2"/>
       <c r="AH32" s="2"/>
       <c r="AI32" s="2"/>
-      <c r="AJ32" s="6"/>
-      <c r="AK32" s="6"/>
+      <c r="AJ32" s="5"/>
+      <c r="AK32" s="5"/>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A33" s="11">
+      <c r="A33" s="10">
         <v>29</v>
       </c>
       <c r="B33" s="2">
         <v>38700</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <v>40200</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="3">
         <v>43300</v>
       </c>
       <c r="E33" s="2">
@@ -4015,7 +4027,7 @@
       <c r="O33" s="2">
         <v>79000</v>
       </c>
-      <c r="P33" s="19">
+      <c r="P33" s="18">
         <v>95700</v>
       </c>
       <c r="Q33" s="2">
@@ -4061,20 +4073,20 @@
       <c r="AG33" s="2"/>
       <c r="AH33" s="2"/>
       <c r="AI33" s="2"/>
-      <c r="AJ33" s="6"/>
-      <c r="AK33" s="6"/>
+      <c r="AJ33" s="5"/>
+      <c r="AK33" s="5"/>
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A34" s="11">
+      <c r="A34" s="10">
         <v>30</v>
       </c>
       <c r="B34" s="2">
         <v>39900</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="3">
         <v>41400</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="3">
         <v>44600</v>
       </c>
       <c r="E34" s="2">
@@ -4110,7 +4122,7 @@
       <c r="O34" s="2">
         <v>81400</v>
       </c>
-      <c r="P34" s="19">
+      <c r="P34" s="18">
         <v>98600</v>
       </c>
       <c r="Q34" s="2">
@@ -4156,20 +4168,20 @@
       <c r="AG34" s="2"/>
       <c r="AH34" s="2"/>
       <c r="AI34" s="2"/>
-      <c r="AJ34" s="6"/>
-      <c r="AK34" s="6"/>
+      <c r="AJ34" s="5"/>
+      <c r="AK34" s="5"/>
     </row>
     <row r="35" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A35" s="11">
+      <c r="A35" s="10">
         <v>31</v>
       </c>
       <c r="B35" s="2">
         <v>41100</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="3">
         <v>42600</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="3">
         <v>45900</v>
       </c>
       <c r="E35" s="2">
@@ -4205,7 +4217,7 @@
       <c r="O35" s="2">
         <v>83800</v>
       </c>
-      <c r="P35" s="19">
+      <c r="P35" s="18">
         <v>101600</v>
       </c>
       <c r="Q35" s="2">
@@ -4251,20 +4263,20 @@
       <c r="AG35" s="2"/>
       <c r="AH35" s="2"/>
       <c r="AI35" s="2"/>
-      <c r="AJ35" s="6"/>
-      <c r="AK35" s="6"/>
+      <c r="AJ35" s="5"/>
+      <c r="AK35" s="5"/>
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A36" s="11">
+      <c r="A36" s="10">
         <v>32</v>
       </c>
       <c r="B36" s="2">
         <v>42300</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="3">
         <v>43900</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="3">
         <v>47300</v>
       </c>
       <c r="E36" s="2">
@@ -4300,7 +4312,7 @@
       <c r="O36" s="2">
         <v>86300</v>
       </c>
-      <c r="P36" s="19">
+      <c r="P36" s="18">
         <v>104600</v>
       </c>
       <c r="Q36" s="2">
@@ -4346,20 +4358,20 @@
       <c r="AG36" s="2"/>
       <c r="AH36" s="2"/>
       <c r="AI36" s="2"/>
-      <c r="AJ36" s="6"/>
-      <c r="AK36" s="6"/>
+      <c r="AJ36" s="5"/>
+      <c r="AK36" s="5"/>
     </row>
     <row r="37" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A37" s="11">
+      <c r="A37" s="10">
         <v>33</v>
       </c>
       <c r="B37" s="2">
         <v>43600</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="3">
         <v>45200</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="3">
         <v>48700</v>
       </c>
       <c r="E37" s="2">
@@ -4395,7 +4407,7 @@
       <c r="O37" s="2">
         <v>88900</v>
       </c>
-      <c r="P37" s="19">
+      <c r="P37" s="18">
         <v>107700</v>
       </c>
       <c r="Q37" s="2">
@@ -4441,62 +4453,67 @@
       <c r="AG37" s="2"/>
       <c r="AH37" s="2"/>
       <c r="AI37" s="2"/>
-      <c r="AJ37" s="6"/>
-      <c r="AK37" s="6"/>
+      <c r="AJ37" s="5"/>
+      <c r="AK37" s="5"/>
     </row>
     <row r="41" spans="1:37" ht="21" x14ac:dyDescent="0.35">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="16"/>
-      <c r="J41" s="16"/>
-      <c r="K41" s="16"/>
-      <c r="L41" s="16"/>
-      <c r="M41" s="16"/>
-      <c r="N41" s="16"/>
-      <c r="O41" s="16"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
     </row>
     <row r="42" spans="1:37" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:37" ht="21" x14ac:dyDescent="0.35">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="17"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="17"/>
-      <c r="K43" s="17"/>
-      <c r="L43" s="17"/>
-      <c r="M43" s="17"/>
-      <c r="N43" s="17"/>
-      <c r="O43" s="17"/>
-      <c r="P43" s="17"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="16"/>
+      <c r="O43" s="16"/>
+      <c r="P43" s="16"/>
     </row>
-    <row r="44" spans="1:37" ht="21" x14ac:dyDescent="0.25">
-      <c r="A44" s="20" t="s">
-        <v>16</v>
+    <row r="44" spans="1:37" ht="21" x14ac:dyDescent="0.3">
+      <c r="A44" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="K44" s="21" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:37" ht="21" x14ac:dyDescent="0.35">
-      <c r="A45" s="21" t="s">
-        <v>17</v>
+      <c r="A45" s="20" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9LuyOdcMze0fY3baskUDELysjZPImuKScbdX2bI0ugCQ1W4AHGWz2VlfbiDky/UwzzOHhi+oG0PofVvTxd+rOQ==" saltValue="/I7s7yc48+JafksyUpFyCw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <hyperlinks>
+    <hyperlink ref="K44" r:id="rId1" tooltip="Click Here to Download" xr:uid="{9C572E2C-328D-460D-9FBF-80AC34D247DF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>